<commit_message>
release for Murkmire (API bump)
</commit_message>
<xml_diff>
--- a/CPData.xlsx
+++ b/CPData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk-mi\Documents\ESOdev\Constellations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8312FF3-F9A9-4C40-AD9C-01D303EA4E21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33260B0-CE26-4AA3-9E62-22B3CC50A2AA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="481">
   <si>
     <t>Points</t>
   </si>
@@ -1482,6 +1487,9 @@
   </si>
   <si>
     <t>Master - at - Arms</t>
+  </si>
+  <si>
+    <t>Radiant Glory</t>
   </si>
 </sst>
 </file>
@@ -15888,7 +15896,7 @@
         <v>3754</v>
       </c>
       <c r="G175" s="24">
-        <f t="shared" ref="G175:G190" si="13">F175/E175/N$2/1.52-1</f>
+        <f t="shared" ref="G175:G187" si="13">F175/E175/N$2/1.52-1</f>
         <v>4.9691909359750541E-2</v>
       </c>
       <c r="H175" t="b">
@@ -16514,7 +16522,7 @@
         <v>3248</v>
       </c>
       <c r="G194" s="24">
-        <f t="shared" ref="G194:G196" si="14">F194/E194/N$196-1</f>
+        <f t="shared" ref="G194:G195" si="14">F194/E194/N$196-1</f>
         <v>4.9728463186821115E-2</v>
       </c>
       <c r="H194" t="b">
@@ -16664,8 +16672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K1137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K435"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K436" sqref="K5:K436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16777,7 +16785,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K3:K66" si="0">CONCATENATE("[",D5,"] = {",LOWER(E5),", ",LOWER(F5),", ",LOWER(G5),", ",LOWER(H5),", ",LOWER(I5),", ",LOWER(J5),"}, --",B5)</f>
+        <f t="shared" ref="K5:K66" si="0">CONCATENATE("[",D5,"] = {",LOWER(E5),", ",LOWER(F5),", ",LOWER(G5),", ",LOWER(H5),", ",LOWER(I5),", ",LOWER(J5),"}, --",B5)</f>
         <v>[40267] = {true, false, true, false, true, true}, --Anti-Calvary Caltrops</v>
       </c>
     </row>
@@ -28702,22 +28710,22 @@
         <v>92</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>24</v>
+        <v>480</v>
       </c>
       <c r="C337" s="12">
-        <v>22182</v>
+        <v>63044</v>
       </c>
       <c r="D337" s="13">
-        <v>22182</v>
+        <v>63956</v>
       </c>
       <c r="E337" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F337" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G337" s="15" t="b">
-        <v>0</v>
+      <c r="F337" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G337" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H337" s="15" t="b">
         <v>0</v>
@@ -28730,7 +28738,7 @@
       </c>
       <c r="K337" t="str">
         <f t="shared" si="5"/>
-        <v>[22182] = {true, true, false, false, true, true}, --Radiant Ward</v>
+        <v>[63956] = {true, false, true, false, true, true}, --Radiant Glory</v>
       </c>
     </row>
     <row r="338" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28738,13 +28746,13 @@
         <v>92</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C338" s="12">
-        <v>21732</v>
+        <v>22182</v>
       </c>
       <c r="D338" s="13">
-        <v>21732</v>
+        <v>22182</v>
       </c>
       <c r="E338" s="14" t="b">
         <v>1</v>
@@ -28766,7 +28774,7 @@
       </c>
       <c r="K338" t="str">
         <f t="shared" si="5"/>
-        <v>[21732] = {true, true, false, false, true, true}, --Reflective Light</v>
+        <v>[22182] = {true, true, false, false, true, true}, --Radiant Ward</v>
       </c>
     </row>
     <row r="339" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28774,22 +28782,22 @@
         <v>92</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C339" s="12">
         <v>21732</v>
       </c>
       <c r="D339" s="13">
-        <v>21734</v>
+        <v>21732</v>
       </c>
       <c r="E339" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F339" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G339" s="14" t="b">
-        <v>1</v>
+      <c r="F339" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G339" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H339" s="15" t="b">
         <v>0</v>
@@ -28802,7 +28810,7 @@
       </c>
       <c r="K339" t="str">
         <f t="shared" si="5"/>
-        <v>[21734] = {true, false, true, false, true, true}, --Reflective Light (dot)</v>
+        <v>[21732] = {true, true, false, false, true, true}, --Reflective Light</v>
       </c>
     </row>
     <row r="340" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28810,13 +28818,13 @@
         <v>92</v>
       </c>
       <c r="B340" s="11" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C340" s="12">
-        <v>22259</v>
+        <v>21732</v>
       </c>
       <c r="D340" s="13">
-        <v>80172</v>
+        <v>21734</v>
       </c>
       <c r="E340" s="14" t="b">
         <v>1</v>
@@ -28838,7 +28846,7 @@
       </c>
       <c r="K340" t="str">
         <f t="shared" si="5"/>
-        <v>[80172] = {true, false, true, false, true, true}, --Ritual of Retribution</v>
+        <v>[21734] = {true, false, true, false, true, true}, --Reflective Light (dot)</v>
       </c>
     </row>
     <row r="341" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28846,22 +28854,22 @@
         <v>92</v>
       </c>
       <c r="B341" s="11" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="C341" s="12">
-        <v>22095</v>
+        <v>22259</v>
       </c>
       <c r="D341" s="13">
-        <v>100218</v>
+        <v>80172</v>
       </c>
       <c r="E341" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F341" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G341" s="15" t="b">
-        <v>0</v>
+      <c r="F341" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G341" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H341" s="15" t="b">
         <v>0</v>
@@ -28874,7 +28882,7 @@
       </c>
       <c r="K341" t="str">
         <f t="shared" si="5"/>
-        <v>[100218] = {true, true, false, false, true, true}, --Solar Barrage</v>
+        <v>[80172] = {true, false, true, false, true, true}, --Ritual of Retribution</v>
       </c>
     </row>
     <row r="342" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28882,22 +28890,22 @@
         <v>92</v>
       </c>
       <c r="B342" s="11" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="C342" s="12">
-        <v>21758</v>
+        <v>22095</v>
       </c>
       <c r="D342" s="13">
-        <v>21759</v>
+        <v>100218</v>
       </c>
       <c r="E342" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F342" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G342" s="14" t="b">
-        <v>1</v>
+      <c r="F342" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G342" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H342" s="15" t="b">
         <v>0</v>
@@ -28910,7 +28918,7 @@
       </c>
       <c r="K342" t="str">
         <f t="shared" si="5"/>
-        <v>[21759] = {true, false, true, false, true, true}, --Solar Disturbance</v>
+        <v>[100218] = {true, true, false, false, true, true}, --Solar Barrage</v>
       </c>
     </row>
     <row r="343" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28918,13 +28926,13 @@
         <v>92</v>
       </c>
       <c r="B343" s="11" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="C343" s="12">
-        <v>21755</v>
+        <v>21758</v>
       </c>
       <c r="D343" s="13">
-        <v>21756</v>
+        <v>21759</v>
       </c>
       <c r="E343" s="14" t="b">
         <v>1</v>
@@ -28946,7 +28954,7 @@
       </c>
       <c r="K343" t="str">
         <f t="shared" si="5"/>
-        <v>[21756] = {true, false, true, false, true, true}, --Solar Prison</v>
+        <v>[21759] = {true, false, true, false, true, true}, --Solar Disturbance</v>
       </c>
     </row>
     <row r="344" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28954,22 +28962,22 @@
         <v>92</v>
       </c>
       <c r="B344" s="11" t="s">
-        <v>385</v>
+        <v>78</v>
       </c>
       <c r="C344" s="12">
-        <v>21726</v>
+        <v>21755</v>
       </c>
       <c r="D344" s="13">
-        <v>21726</v>
+        <v>21756</v>
       </c>
       <c r="E344" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F344" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G344" s="15" t="b">
-        <v>0</v>
+      <c r="F344" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G344" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H344" s="15" t="b">
         <v>0</v>
@@ -28982,7 +28990,7 @@
       </c>
       <c r="K344" t="str">
         <f t="shared" si="5"/>
-        <v>[21726] = {true, true, false, false, true, true}, --Sun Fire</v>
+        <v>[21756] = {true, false, true, false, true, true}, --Solar Prison</v>
       </c>
     </row>
     <row r="345" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28990,22 +28998,22 @@
         <v>92</v>
       </c>
       <c r="B345" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C345" s="12">
         <v>21726</v>
       </c>
       <c r="D345" s="13">
-        <v>21728</v>
+        <v>21726</v>
       </c>
       <c r="E345" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F345" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G345" s="14" t="b">
-        <v>1</v>
+      <c r="F345" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G345" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H345" s="15" t="b">
         <v>0</v>
@@ -29018,7 +29026,7 @@
       </c>
       <c r="K345" t="str">
         <f t="shared" si="5"/>
-        <v>[21728] = {true, false, true, false, true, true}, --Sun Fire (DoT)</v>
+        <v>[21726] = {true, true, false, false, true, true}, --Sun Fire</v>
       </c>
     </row>
     <row r="346" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29026,22 +29034,22 @@
         <v>92</v>
       </c>
       <c r="B346" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C346" s="12">
-        <v>22178</v>
+        <v>21726</v>
       </c>
       <c r="D346" s="13">
-        <v>22178</v>
+        <v>21728</v>
       </c>
       <c r="E346" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F346" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G346" s="15" t="b">
-        <v>0</v>
+      <c r="F346" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G346" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H346" s="15" t="b">
         <v>0</v>
@@ -29054,7 +29062,7 @@
       </c>
       <c r="K346" t="str">
         <f t="shared" si="5"/>
-        <v>[22178] = {true, true, false, false, true, true}, --Sun Shield</v>
+        <v>[21728] = {true, false, true, false, true, true}, --Sun Fire (DoT)</v>
       </c>
     </row>
     <row r="347" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29062,13 +29070,13 @@
         <v>92</v>
       </c>
       <c r="B347" s="11" t="s">
-        <v>133</v>
+        <v>387</v>
       </c>
       <c r="C347" s="12">
-        <v>15540</v>
+        <v>22178</v>
       </c>
       <c r="D347" s="13">
-        <v>15544</v>
+        <v>22178</v>
       </c>
       <c r="E347" s="14" t="b">
         <v>1</v>
@@ -29090,7 +29098,7 @@
       </c>
       <c r="K347" t="str">
         <f t="shared" si="5"/>
-        <v>[15544] = {true, true, false, false, true, true}, --Toppling Charge</v>
+        <v>[22178] = {true, true, false, false, true, true}, --Sun Shield</v>
       </c>
     </row>
     <row r="348" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29098,13 +29106,13 @@
         <v>92</v>
       </c>
       <c r="B348" s="11" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C348" s="12">
-        <v>22006</v>
+        <v>15540</v>
       </c>
       <c r="D348" s="13">
-        <v>68729</v>
+        <v>15544</v>
       </c>
       <c r="E348" s="14" t="b">
         <v>1</v>
@@ -29126,7 +29134,7 @@
       </c>
       <c r="K348" t="str">
         <f t="shared" si="5"/>
-        <v>[68729] = {true, true, false, false, true, true}, --Total Dark</v>
+        <v>[15544] = {true, true, false, false, true, true}, --Toppling Charge</v>
       </c>
     </row>
     <row r="349" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29134,13 +29142,13 @@
         <v>92</v>
       </c>
       <c r="B349" s="11" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="C349" s="12">
-        <v>22004</v>
+        <v>22006</v>
       </c>
       <c r="D349" s="13">
-        <v>22005</v>
+        <v>68729</v>
       </c>
       <c r="E349" s="14" t="b">
         <v>1</v>
@@ -29162,7 +29170,7 @@
       </c>
       <c r="K349" t="str">
         <f t="shared" si="5"/>
-        <v>[22005] = {true, true, false, false, true, true}, --Unstable Core</v>
+        <v>[68729] = {true, true, false, false, true, true}, --Total Dark</v>
       </c>
     </row>
     <row r="350" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29170,13 +29178,13 @@
         <v>92</v>
       </c>
       <c r="B350" s="11" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="C350" s="12">
-        <v>21729</v>
+        <v>22004</v>
       </c>
       <c r="D350" s="13">
-        <v>21729</v>
+        <v>22005</v>
       </c>
       <c r="E350" s="14" t="b">
         <v>1</v>
@@ -29198,7 +29206,7 @@
       </c>
       <c r="K350" t="str">
         <f t="shared" si="5"/>
-        <v>[21729] = {true, true, false, false, true, true}, --Vampires Bane</v>
+        <v>[22005] = {true, true, false, false, true, true}, --Unstable Core</v>
       </c>
     </row>
     <row r="351" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29206,22 +29214,22 @@
         <v>92</v>
       </c>
       <c r="B351" s="11" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C351" s="12">
         <v>21729</v>
       </c>
       <c r="D351" s="13">
-        <v>21731</v>
+        <v>21729</v>
       </c>
       <c r="E351" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F351" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G351" s="14" t="b">
-        <v>1</v>
+      <c r="F351" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G351" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H351" s="15" t="b">
         <v>0</v>
@@ -29234,30 +29242,30 @@
       </c>
       <c r="K351" t="str">
         <f t="shared" si="5"/>
-        <v>[21731] = {true, false, true, false, true, true}, --Vampires Bane (dot)</v>
+        <v>[21729] = {true, true, false, false, true, true}, --Vampires Bane</v>
       </c>
     </row>
     <row r="352" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="10" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="B352" s="11" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C352" s="12">
-        <v>83238</v>
+        <v>21729</v>
       </c>
       <c r="D352" s="13">
-        <v>83238</v>
+        <v>21731</v>
       </c>
       <c r="E352" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F352" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G352" s="15" t="b">
-        <v>0</v>
+      <c r="F352" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G352" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H352" s="15" t="b">
         <v>0</v>
@@ -29265,12 +29273,12 @@
       <c r="I352" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J352" s="15" t="b">
-        <v>0</v>
+      <c r="J352" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K352" t="str">
         <f t="shared" si="5"/>
-        <v>[83238] = {true, true, false, false, true, false}, --Berserker Rage</v>
+        <v>[21731] = {true, false, true, false, true, true}, --Vampires Bane (dot)</v>
       </c>
     </row>
     <row r="353" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29278,13 +29286,13 @@
         <v>139</v>
       </c>
       <c r="B353" s="11" t="s">
-        <v>393</v>
+        <v>144</v>
       </c>
       <c r="C353" s="12">
-        <v>83216</v>
+        <v>83238</v>
       </c>
       <c r="D353" s="13">
-        <v>83216</v>
+        <v>83238</v>
       </c>
       <c r="E353" s="14" t="b">
         <v>1</v>
@@ -29306,7 +29314,7 @@
       </c>
       <c r="K353" t="str">
         <f t="shared" si="5"/>
-        <v>[83216] = {true, true, false, false, true, false}, --Berserker Strike</v>
+        <v>[83238] = {true, true, false, false, true, false}, --Berserker Rage</v>
       </c>
     </row>
     <row r="354" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29314,13 +29322,13 @@
         <v>139</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>154</v>
+        <v>393</v>
       </c>
       <c r="C354" s="12">
-        <v>38754</v>
+        <v>83216</v>
       </c>
       <c r="D354" s="13">
-        <v>38754</v>
+        <v>83216</v>
       </c>
       <c r="E354" s="14" t="b">
         <v>1</v>
@@ -29337,12 +29345,12 @@
       <c r="I354" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J354" s="14" t="b">
-        <v>1</v>
+      <c r="J354" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K354" t="str">
         <f t="shared" si="5"/>
-        <v>[38754] = {true, true, false, false, true, true}, --Brawler</v>
+        <v>[83216] = {true, true, false, false, true, false}, --Berserker Strike</v>
       </c>
     </row>
     <row r="355" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29350,22 +29358,22 @@
         <v>139</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C355" s="12">
         <v>38754</v>
       </c>
       <c r="D355" s="13">
-        <v>38759</v>
+        <v>38754</v>
       </c>
       <c r="E355" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F355" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G355" s="14" t="b">
-        <v>1</v>
+      <c r="F355" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G355" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H355" s="15" t="b">
         <v>0</v>
@@ -29373,12 +29381,12 @@
       <c r="I355" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J355" s="15" t="b">
-        <v>0</v>
+      <c r="J355" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K355" t="str">
         <f t="shared" si="5"/>
-        <v>[38759] = {true, false, true, false, true, false}, --Brawler Bleed</v>
+        <v>[38754] = {true, true, false, false, true, true}, --Brawler</v>
       </c>
     </row>
     <row r="356" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29386,22 +29394,22 @@
         <v>139</v>
       </c>
       <c r="B356" s="11" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C356" s="12">
-        <v>38745</v>
+        <v>38754</v>
       </c>
       <c r="D356" s="13">
-        <v>38745</v>
+        <v>38759</v>
       </c>
       <c r="E356" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F356" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G356" s="15" t="b">
-        <v>0</v>
+      <c r="F356" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G356" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H356" s="15" t="b">
         <v>0</v>
@@ -29409,12 +29417,12 @@
       <c r="I356" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J356" s="14" t="b">
-        <v>1</v>
+      <c r="J356" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K356" t="str">
         <f t="shared" si="5"/>
-        <v>[38745] = {true, true, false, false, true, true}, --Carve</v>
+        <v>[38759] = {true, false, true, false, true, false}, --Brawler Bleed</v>
       </c>
     </row>
     <row r="357" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29422,22 +29430,22 @@
         <v>139</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C357" s="12">
         <v>38745</v>
       </c>
       <c r="D357" s="13">
-        <v>38747</v>
+        <v>38745</v>
       </c>
       <c r="E357" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F357" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G357" s="14" t="b">
-        <v>1</v>
+      <c r="F357" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G357" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H357" s="15" t="b">
         <v>0</v>
@@ -29445,12 +29453,12 @@
       <c r="I357" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J357" s="15" t="b">
-        <v>0</v>
+      <c r="J357" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K357" t="str">
         <f t="shared" si="5"/>
-        <v>[38747] = {true, false, true, false, true, false}, --Carve Bleed</v>
+        <v>[38745] = {true, true, false, false, true, true}, --Carve</v>
       </c>
     </row>
     <row r="358" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29458,22 +29466,22 @@
         <v>139</v>
       </c>
       <c r="B358" s="11" t="s">
-        <v>390</v>
+        <v>106</v>
       </c>
       <c r="C358" s="12">
-        <v>20919</v>
+        <v>38745</v>
       </c>
       <c r="D358" s="13">
-        <v>20919</v>
+        <v>38747</v>
       </c>
       <c r="E358" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F358" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G358" s="15" t="b">
-        <v>0</v>
+      <c r="F358" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G358" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H358" s="15" t="b">
         <v>0</v>
@@ -29481,12 +29489,12 @@
       <c r="I358" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J358" s="14" t="b">
-        <v>1</v>
+      <c r="J358" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K358" t="str">
         <f t="shared" si="5"/>
-        <v>[20919] = {true, true, false, false, true, true}, --Cleave</v>
+        <v>[38747] = {true, false, true, false, true, false}, --Carve Bleed</v>
       </c>
     </row>
     <row r="359" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29494,22 +29502,22 @@
         <v>139</v>
       </c>
       <c r="B359" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C359" s="12">
         <v>20919</v>
       </c>
       <c r="D359" s="13">
-        <v>31059</v>
+        <v>20919</v>
       </c>
       <c r="E359" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F359" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G359" s="14" t="b">
-        <v>1</v>
+      <c r="F359" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G359" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H359" s="15" t="b">
         <v>0</v>
@@ -29517,12 +29525,12 @@
       <c r="I359" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J359" s="15" t="b">
-        <v>0</v>
+      <c r="J359" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K359" t="str">
         <f t="shared" si="5"/>
-        <v>[31059] = {true, false, true, false, true, false}, --Cleave Bleed</v>
+        <v>[20919] = {true, true, false, false, true, true}, --Cleave</v>
       </c>
     </row>
     <row r="360" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29530,22 +29538,22 @@
         <v>139</v>
       </c>
       <c r="B360" s="11" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C360" s="12">
-        <v>28448</v>
+        <v>20919</v>
       </c>
       <c r="D360" s="13">
-        <v>28449</v>
+        <v>31059</v>
       </c>
       <c r="E360" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F360" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G360" s="15" t="b">
-        <v>0</v>
+      <c r="F360" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G360" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H360" s="15" t="b">
         <v>0</v>
@@ -29553,12 +29561,12 @@
       <c r="I360" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J360" s="14" t="b">
-        <v>1</v>
+      <c r="J360" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K360" t="str">
         <f t="shared" si="5"/>
-        <v>[28449] = {true, true, false, false, true, true}, --Critical Charge</v>
+        <v>[31059] = {true, false, true, false, true, false}, --Cleave Bleed</v>
       </c>
     </row>
     <row r="361" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29566,13 +29574,13 @@
         <v>139</v>
       </c>
       <c r="B361" s="11" t="s">
-        <v>145</v>
+        <v>389</v>
       </c>
       <c r="C361" s="12">
-        <v>38778</v>
+        <v>28448</v>
       </c>
       <c r="D361" s="13">
-        <v>38782</v>
+        <v>28449</v>
       </c>
       <c r="E361" s="14" t="b">
         <v>1</v>
@@ -29594,7 +29602,7 @@
       </c>
       <c r="K361" t="str">
         <f t="shared" si="5"/>
-        <v>[38782] = {true, true, false, false, true, true}, --Critical Rush</v>
+        <v>[28449] = {true, true, false, false, true, true}, --Critical Charge</v>
       </c>
     </row>
     <row r="362" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29602,13 +29610,13 @@
         <v>139</v>
       </c>
       <c r="B362" s="11" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="C362" s="12">
-        <v>38814</v>
+        <v>38778</v>
       </c>
       <c r="D362" s="13">
-        <v>38814</v>
+        <v>38782</v>
       </c>
       <c r="E362" s="14" t="b">
         <v>1</v>
@@ -29630,7 +29638,7 @@
       </c>
       <c r="K362" t="str">
         <f t="shared" si="5"/>
-        <v>[38814] = {true, true, false, false, true, true}, --Dizzying Swing</v>
+        <v>[38782] = {true, true, false, false, true, true}, --Critical Rush</v>
       </c>
     </row>
     <row r="363" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29638,13 +29646,13 @@
         <v>139</v>
       </c>
       <c r="B363" s="11" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="C363" s="12">
-        <v>38819</v>
+        <v>38814</v>
       </c>
       <c r="D363" s="13">
-        <v>38819</v>
+        <v>38814</v>
       </c>
       <c r="E363" s="14" t="b">
         <v>1</v>
@@ -29666,7 +29674,7 @@
       </c>
       <c r="K363" t="str">
         <f t="shared" si="5"/>
-        <v>[38819] = {true, true, false, false, true, true}, --Executioner</v>
+        <v>[38814] = {true, true, false, false, true, true}, --Dizzying Swing</v>
       </c>
     </row>
     <row r="364" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29674,13 +29682,13 @@
         <v>139</v>
       </c>
       <c r="B364" s="11" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="C364" s="12">
-        <v>16041</v>
+        <v>38819</v>
       </c>
       <c r="D364" s="13">
-        <v>17163</v>
+        <v>38819</v>
       </c>
       <c r="E364" s="14" t="b">
         <v>1</v>
@@ -29691,8 +29699,8 @@
       <c r="G364" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H364" s="14" t="b">
-        <v>1</v>
+      <c r="H364" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="I364" s="14" t="b">
         <v>1</v>
@@ -29702,7 +29710,7 @@
       </c>
       <c r="K364" t="str">
         <f t="shared" si="5"/>
-        <v>[17163] = {true, true, false, true, true, true}, --Heavy Attack (2H)</v>
+        <v>[38819] = {true, true, false, false, true, true}, --Executioner</v>
       </c>
     </row>
     <row r="365" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29710,13 +29718,13 @@
         <v>139</v>
       </c>
       <c r="B365" s="11" t="s">
-        <v>444</v>
+        <v>129</v>
       </c>
       <c r="C365" s="12">
         <v>16041</v>
       </c>
       <c r="D365" s="13">
-        <v>17162</v>
+        <v>17163</v>
       </c>
       <c r="E365" s="14" t="b">
         <v>1</v>
@@ -29738,7 +29746,7 @@
       </c>
       <c r="K365" t="str">
         <f t="shared" si="5"/>
-        <v>[17162] = {true, true, false, true, true, true}, --Heavy Attack (Medium, 2H)</v>
+        <v>[17163] = {true, true, false, true, true, true}, --Heavy Attack (2H)</v>
       </c>
     </row>
     <row r="366" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29746,35 +29754,35 @@
         <v>139</v>
       </c>
       <c r="B366" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="C366" s="12" t="s">
-        <v>33</v>
+        <v>444</v>
+      </c>
+      <c r="C366" s="12">
+        <v>16041</v>
       </c>
       <c r="D366" s="13">
-        <v>45431</v>
+        <v>17162</v>
       </c>
       <c r="E366" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F366" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G366" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H366" s="15" t="b">
-        <v>0</v>
+      <c r="F366" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G366" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H366" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="I366" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J366" s="15" t="b">
-        <v>0</v>
+      <c r="J366" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K366" t="str">
         <f t="shared" si="5"/>
-        <v>[45431] = {true, false, true, false, true, false}, --Heavy Weapons Bleed</v>
+        <v>[17162] = {true, true, false, true, true, true}, --Heavy Attack (Medium, 2H)</v>
       </c>
     </row>
     <row r="367" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29782,35 +29790,35 @@
         <v>139</v>
       </c>
       <c r="B367" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C367" s="12">
-        <v>16037</v>
+        <v>394</v>
+      </c>
+      <c r="C367" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D367" s="13">
-        <v>16037</v>
+        <v>45431</v>
       </c>
       <c r="E367" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F367" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G367" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H367" s="14" t="b">
-        <v>1</v>
+      <c r="F367" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G367" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H367" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="I367" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J367" s="14" t="b">
-        <v>1</v>
+      <c r="J367" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K367" t="str">
         <f t="shared" si="5"/>
-        <v>[16037] = {true, true, false, true, true, true}, --Light Attack (2H)</v>
+        <v>[45431] = {true, false, true, false, true, false}, --Heavy Weapons Bleed</v>
       </c>
     </row>
     <row r="368" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29818,13 +29826,13 @@
         <v>139</v>
       </c>
       <c r="B368" s="11" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C368" s="12">
-        <v>83229</v>
+        <v>16037</v>
       </c>
       <c r="D368" s="13">
-        <v>83229</v>
+        <v>16037</v>
       </c>
       <c r="E368" s="14" t="b">
         <v>1</v>
@@ -29835,18 +29843,18 @@
       <c r="G368" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H368" s="15" t="b">
-        <v>0</v>
+      <c r="H368" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="I368" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J368" s="15" t="b">
-        <v>0</v>
+      <c r="J368" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K368" t="str">
         <f t="shared" si="5"/>
-        <v>[83229] = {true, true, false, false, true, false}, --Onslaught</v>
+        <v>[16037] = {true, true, false, true, true, true}, --Light Attack (2H)</v>
       </c>
     </row>
     <row r="369" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29854,13 +29862,13 @@
         <v>139</v>
       </c>
       <c r="B369" s="11" t="s">
-        <v>392</v>
+        <v>114</v>
       </c>
       <c r="C369" s="12">
-        <v>28302</v>
+        <v>83229</v>
       </c>
       <c r="D369" s="13">
-        <v>28302</v>
+        <v>83229</v>
       </c>
       <c r="E369" s="14" t="b">
         <v>1</v>
@@ -29877,12 +29885,12 @@
       <c r="I369" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J369" s="14" t="b">
-        <v>1</v>
+      <c r="J369" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K369" t="str">
         <f t="shared" si="5"/>
-        <v>[28302] = {true, true, false, false, true, true}, --Reverse Slash</v>
+        <v>[83229] = {true, true, false, false, true, false}, --Onslaught</v>
       </c>
     </row>
     <row r="370" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29890,13 +29898,13 @@
         <v>139</v>
       </c>
       <c r="B370" s="11" t="s">
-        <v>110</v>
+        <v>392</v>
       </c>
       <c r="C370" s="12">
-        <v>38823</v>
+        <v>28302</v>
       </c>
       <c r="D370" s="13">
-        <v>38823</v>
+        <v>28302</v>
       </c>
       <c r="E370" s="14" t="b">
         <v>1</v>
@@ -29918,7 +29926,7 @@
       </c>
       <c r="K370" t="str">
         <f t="shared" si="5"/>
-        <v>[38823] = {true, true, false, false, true, true}, --Reverse Slice</v>
+        <v>[28302] = {true, true, false, false, true, true}, --Reverse Slash</v>
       </c>
     </row>
     <row r="371" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29926,13 +29934,13 @@
         <v>139</v>
       </c>
       <c r="B371" s="11" t="s">
-        <v>395</v>
+        <v>110</v>
       </c>
       <c r="C371" s="12">
         <v>38823</v>
       </c>
       <c r="D371" s="13">
-        <v>38827</v>
+        <v>38823</v>
       </c>
       <c r="E371" s="14" t="b">
         <v>1</v>
@@ -29954,7 +29962,7 @@
       </c>
       <c r="K371" t="str">
         <f t="shared" si="5"/>
-        <v>[38827] = {true, true, false, false, true, true}, --Reverse Slice (2nd)</v>
+        <v>[38823] = {true, true, false, false, true, true}, --Reverse Slice</v>
       </c>
     </row>
     <row r="372" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29962,13 +29970,13 @@
         <v>139</v>
       </c>
       <c r="B372" s="11" t="s">
-        <v>108</v>
+        <v>395</v>
       </c>
       <c r="C372" s="12">
-        <v>38788</v>
+        <v>38823</v>
       </c>
       <c r="D372" s="13">
-        <v>38792</v>
+        <v>38827</v>
       </c>
       <c r="E372" s="14" t="b">
         <v>1</v>
@@ -29990,7 +29998,7 @@
       </c>
       <c r="K372" t="str">
         <f t="shared" si="5"/>
-        <v>[38792] = {true, true, false, false, true, true}, --Stampede</v>
+        <v>[38827] = {true, true, false, false, true, true}, --Reverse Slice (2nd)</v>
       </c>
     </row>
     <row r="373" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29998,13 +30006,13 @@
         <v>139</v>
       </c>
       <c r="B373" s="11" t="s">
-        <v>388</v>
+        <v>108</v>
       </c>
       <c r="C373" s="12">
-        <v>28279</v>
+        <v>38788</v>
       </c>
       <c r="D373" s="13">
-        <v>28279</v>
+        <v>38792</v>
       </c>
       <c r="E373" s="14" t="b">
         <v>1</v>
@@ -30026,7 +30034,7 @@
       </c>
       <c r="K373" t="str">
         <f t="shared" si="5"/>
-        <v>[28279] = {true, true, false, false, true, true}, --Uppercut</v>
+        <v>[38792] = {true, true, false, false, true, true}, --Stampede</v>
       </c>
     </row>
     <row r="374" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30034,13 +30042,13 @@
         <v>139</v>
       </c>
       <c r="B374" s="11" t="s">
-        <v>146</v>
+        <v>388</v>
       </c>
       <c r="C374" s="12">
-        <v>38807</v>
+        <v>28279</v>
       </c>
       <c r="D374" s="13">
-        <v>38807</v>
+        <v>28279</v>
       </c>
       <c r="E374" s="14" t="b">
         <v>1</v>
@@ -30062,21 +30070,21 @@
       </c>
       <c r="K374" t="str">
         <f t="shared" si="5"/>
-        <v>[38807] = {true, true, false, false, true, true}, --Wrecking Blow</v>
+        <v>[28279] = {true, true, false, false, true, true}, --Uppercut</v>
       </c>
     </row>
     <row r="375" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A375" s="10" t="s">
-        <v>396</v>
+        <v>139</v>
       </c>
       <c r="B375" s="11" t="s">
-        <v>397</v>
+        <v>146</v>
       </c>
       <c r="C375" s="12">
-        <v>42060</v>
+        <v>38807</v>
       </c>
       <c r="D375" s="13">
-        <v>42060</v>
+        <v>38807</v>
       </c>
       <c r="E375" s="14" t="b">
         <v>1</v>
@@ -30098,7 +30106,7 @@
       </c>
       <c r="K375" t="str">
         <f t="shared" si="5"/>
-        <v>[42060] = {true, true, false, false, true, true}, --Inner Beast</v>
+        <v>[38807] = {true, true, false, false, true, true}, --Wrecking Blow</v>
       </c>
     </row>
     <row r="376" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30106,13 +30114,13 @@
         <v>396</v>
       </c>
       <c r="B376" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C376" s="12">
-        <v>42056</v>
+        <v>42060</v>
       </c>
       <c r="D376" s="13">
-        <v>42056</v>
+        <v>42060</v>
       </c>
       <c r="E376" s="14" t="b">
         <v>1</v>
@@ -30134,7 +30142,7 @@
       </c>
       <c r="K376" t="str">
         <f t="shared" si="5"/>
-        <v>[42056] = {true, true, false, false, true, true}, --Inner Rage</v>
+        <v>[42060] = {true, true, false, false, true, true}, --Inner Beast</v>
       </c>
     </row>
     <row r="377" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30142,13 +30150,13 @@
         <v>396</v>
       </c>
       <c r="B377" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C377" s="12">
-        <v>41990</v>
+        <v>42056</v>
       </c>
       <c r="D377" s="13">
-        <v>80107</v>
+        <v>42056</v>
       </c>
       <c r="E377" s="14" t="b">
         <v>1</v>
@@ -30170,7 +30178,7 @@
       </c>
       <c r="K377" t="str">
         <f t="shared" si="5"/>
-        <v>[80107] = {true, true, false, false, true, true}, --Shadow Silk (not synergy)</v>
+        <v>[42056] = {true, true, false, false, true, true}, --Inner Rage</v>
       </c>
     </row>
     <row r="378" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30178,13 +30186,13 @@
         <v>396</v>
       </c>
       <c r="B378" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C378" s="12">
-        <v>42012</v>
+        <v>41990</v>
       </c>
       <c r="D378" s="13">
-        <v>80129</v>
+        <v>80107</v>
       </c>
       <c r="E378" s="14" t="b">
         <v>1</v>
@@ -30206,30 +30214,30 @@
       </c>
       <c r="K378" t="str">
         <f t="shared" si="5"/>
-        <v>[80129] = {true, true, false, false, true, true}, --Tangling Webs (not synergy)</v>
+        <v>[80107] = {true, true, false, false, true, true}, --Shadow Silk (not synergy)</v>
       </c>
     </row>
     <row r="379" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379" s="10" t="s">
-        <v>276</v>
+        <v>396</v>
       </c>
       <c r="B379" s="11" t="s">
-        <v>277</v>
+        <v>400</v>
       </c>
       <c r="C379" s="12">
-        <v>38956</v>
+        <v>42012</v>
       </c>
       <c r="D379" s="13">
-        <v>38956</v>
+        <v>80129</v>
       </c>
       <c r="E379" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F379" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G379" s="14" t="b">
-        <v>1</v>
+      <c r="F379" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G379" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H379" s="15" t="b">
         <v>0</v>
@@ -30242,7 +30250,7 @@
       </c>
       <c r="K379" t="str">
         <f t="shared" si="5"/>
-        <v>[38956] = {true, false, true, false, true, true}, --Accelerating Drain</v>
+        <v>[80129] = {true, true, false, false, true, true}, --Tangling Webs (not synergy)</v>
       </c>
     </row>
     <row r="380" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30250,13 +30258,13 @@
         <v>276</v>
       </c>
       <c r="B380" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C380" s="12">
-        <v>38965</v>
+        <v>38956</v>
       </c>
       <c r="D380" s="13">
-        <v>38968</v>
+        <v>38956</v>
       </c>
       <c r="E380" s="14" t="b">
         <v>1</v>
@@ -30278,7 +30286,7 @@
       </c>
       <c r="K380" t="str">
         <f t="shared" si="5"/>
-        <v>[38968] = {true, false, true, false, true, true}, --Baleful Mist</v>
+        <v>[38956] = {true, false, true, false, true, true}, --Accelerating Drain</v>
       </c>
     </row>
     <row r="381" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30286,13 +30294,13 @@
         <v>276</v>
       </c>
       <c r="B381" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C381" s="12">
-        <v>32624</v>
+        <v>38965</v>
       </c>
       <c r="D381" s="13">
-        <v>32625</v>
+        <v>38968</v>
       </c>
       <c r="E381" s="14" t="b">
         <v>1</v>
@@ -30314,7 +30322,7 @@
       </c>
       <c r="K381" t="str">
         <f t="shared" si="5"/>
-        <v>[32625] = {true, false, true, false, true, true}, --Bat Swarm</v>
+        <v>[38968] = {true, false, true, false, true, true}, --Baleful Mist</v>
       </c>
     </row>
     <row r="382" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30322,13 +30330,13 @@
         <v>276</v>
       </c>
       <c r="B382" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C382" s="12">
-        <v>38932</v>
+        <v>32624</v>
       </c>
       <c r="D382" s="13">
-        <v>38935</v>
+        <v>32625</v>
       </c>
       <c r="E382" s="14" t="b">
         <v>1</v>
@@ -30350,7 +30358,7 @@
       </c>
       <c r="K382" t="str">
         <f t="shared" si="5"/>
-        <v>[38935] = {true, false, true, false, true, true}, --Clouding Swarm</v>
+        <v>[32625] = {true, false, true, false, true, true}, --Bat Swarm</v>
       </c>
     </row>
     <row r="383" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30358,13 +30366,13 @@
         <v>276</v>
       </c>
       <c r="B383" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C383" s="12">
-        <v>38931</v>
+        <v>38932</v>
       </c>
       <c r="D383" s="13">
-        <v>38934</v>
+        <v>38935</v>
       </c>
       <c r="E383" s="14" t="b">
         <v>1</v>
@@ -30386,7 +30394,7 @@
       </c>
       <c r="K383" t="str">
         <f t="shared" si="5"/>
-        <v>[38934] = {true, false, true, false, true, true}, --Devouring Swarm</v>
+        <v>[38935] = {true, false, true, false, true, true}, --Clouding Swarm</v>
       </c>
     </row>
     <row r="384" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30394,13 +30402,13 @@
         <v>276</v>
       </c>
       <c r="B384" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C384" s="12">
-        <v>32893</v>
+        <v>38931</v>
       </c>
       <c r="D384" s="13">
-        <v>32893</v>
+        <v>38934</v>
       </c>
       <c r="E384" s="14" t="b">
         <v>1</v>
@@ -30422,7 +30430,7 @@
       </c>
       <c r="K384" t="str">
         <f t="shared" si="5"/>
-        <v>[32893] = {true, false, true, false, true, true}, --Drain Essence</v>
+        <v>[38934] = {true, false, true, false, true, true}, --Devouring Swarm</v>
       </c>
     </row>
     <row r="385" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30430,13 +30438,13 @@
         <v>276</v>
       </c>
       <c r="B385" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C385" s="12">
-        <v>38949</v>
+        <v>32893</v>
       </c>
       <c r="D385" s="13">
-        <v>38949</v>
+        <v>32893</v>
       </c>
       <c r="E385" s="14" t="b">
         <v>1</v>
@@ -30458,21 +30466,21 @@
       </c>
       <c r="K385" t="str">
         <f t="shared" si="5"/>
-        <v>[38949] = {true, false, true, false, true, true}, --Invigorating Drain</v>
+        <v>[32893] = {true, false, true, false, true, true}, --Drain Essence</v>
       </c>
     </row>
     <row r="386" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A386" s="10" t="s">
-        <v>93</v>
+        <v>276</v>
       </c>
       <c r="B386" s="11" t="s">
-        <v>80</v>
+        <v>283</v>
       </c>
       <c r="C386" s="12">
-        <v>86156</v>
+        <v>38949</v>
       </c>
       <c r="D386" s="13">
-        <v>87256</v>
+        <v>38949</v>
       </c>
       <c r="E386" s="14" t="b">
         <v>1</v>
@@ -30494,7 +30502,7 @@
       </c>
       <c r="K386" t="str">
         <f t="shared" si="5"/>
-        <v>[87256] = {true, false, true, false, true, true}, --Arctic Blast</v>
+        <v>[38949] = {true, false, true, false, true, true}, --Invigorating Drain</v>
       </c>
     </row>
     <row r="387" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30502,22 +30510,22 @@
         <v>93</v>
       </c>
       <c r="B387" s="11" t="s">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="C387" s="12">
-        <v>85986</v>
+        <v>86156</v>
       </c>
       <c r="D387" s="13">
-        <v>105907</v>
+        <v>87256</v>
       </c>
       <c r="E387" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F387" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G387" s="15" t="b">
-        <v>0</v>
+      <c r="F387" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G387" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H387" s="15" t="b">
         <v>0</v>
@@ -30529,8 +30537,8 @@
         <v>1</v>
       </c>
       <c r="K387" t="str">
-        <f t="shared" ref="K387:K435" si="6">CONCATENATE("[",D387,"] = {",LOWER(E387),", ",LOWER(F387),", ",LOWER(G387),", ",LOWER(H387),", ",LOWER(I387),", ",LOWER(J387),"}, --",B387)</f>
-        <v>[105907] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
+        <f t="shared" ref="K387:K436" si="6">CONCATENATE("[",D387,"] = {",LOWER(E387),", ",LOWER(F387),", ",LOWER(G387),", ",LOWER(H387),", ",LOWER(I387),", ",LOWER(J387),"}, --",B387)</f>
+        <v>[87256] = {true, false, true, false, true, true}, --Arctic Blast</v>
       </c>
     </row>
     <row r="388" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30541,10 +30549,10 @@
         <v>250</v>
       </c>
       <c r="C388" s="12">
-        <v>85982</v>
+        <v>85986</v>
       </c>
       <c r="D388" s="13">
-        <v>89128</v>
+        <v>105907</v>
       </c>
       <c r="E388" s="14" t="b">
         <v>1</v>
@@ -30566,7 +30574,7 @@
       </c>
       <c r="K388" t="str">
         <f t="shared" si="6"/>
-        <v>[89128] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
+        <v>[105907] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
       </c>
     </row>
     <row r="389" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30577,10 +30585,10 @@
         <v>250</v>
       </c>
       <c r="C389" s="12">
-        <v>85990</v>
+        <v>85982</v>
       </c>
       <c r="D389" s="13">
-        <v>89220</v>
+        <v>89128</v>
       </c>
       <c r="E389" s="14" t="b">
         <v>1</v>
@@ -30602,7 +30610,7 @@
       </c>
       <c r="K389" t="str">
         <f t="shared" si="6"/>
-        <v>[89220] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
+        <v>[89128] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
       </c>
     </row>
     <row r="390" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30610,13 +30618,13 @@
         <v>93</v>
       </c>
       <c r="B390" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C390" s="12">
-        <v>85999</v>
+        <v>85990</v>
       </c>
       <c r="D390" s="13">
-        <v>85999</v>
+        <v>89220</v>
       </c>
       <c r="E390" s="14" t="b">
         <v>1</v>
@@ -30638,7 +30646,7 @@
       </c>
       <c r="K390" t="str">
         <f t="shared" si="6"/>
-        <v>[85999] = {true, true, false, false, true, true}, --Cutting Dive</v>
+        <v>[89220] = {true, true, false, false, true, true}, --Crushing Swipe (pet)</v>
       </c>
     </row>
     <row r="391" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30646,13 +30654,13 @@
         <v>93</v>
       </c>
       <c r="B391" s="11" t="s">
-        <v>81</v>
+        <v>251</v>
       </c>
       <c r="C391" s="12">
-        <v>86015</v>
+        <v>85999</v>
       </c>
       <c r="D391" s="13">
-        <v>94424</v>
+        <v>85999</v>
       </c>
       <c r="E391" s="14" t="b">
         <v>1</v>
@@ -30674,7 +30682,7 @@
       </c>
       <c r="K391" t="str">
         <f t="shared" si="6"/>
-        <v>[94424] = {true, true, false, false, true, true}, --Deep Fissure</v>
+        <v>[85999] = {true, true, false, false, true, true}, --Cutting Dive</v>
       </c>
     </row>
     <row r="392" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30682,13 +30690,13 @@
         <v>93</v>
       </c>
       <c r="B392" s="11" t="s">
-        <v>401</v>
+        <v>81</v>
       </c>
       <c r="C392" s="12">
-        <v>85995</v>
+        <v>86015</v>
       </c>
       <c r="D392" s="13">
-        <v>85995</v>
+        <v>94424</v>
       </c>
       <c r="E392" s="14" t="b">
         <v>1</v>
@@ -30710,7 +30718,7 @@
       </c>
       <c r="K392" t="str">
         <f t="shared" si="6"/>
-        <v>[85995] = {true, true, false, false, true, true}, --Dive</v>
+        <v>[94424] = {true, true, false, false, true, true}, --Deep Fissure</v>
       </c>
     </row>
     <row r="393" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30718,13 +30726,13 @@
         <v>93</v>
       </c>
       <c r="B393" s="11" t="s">
-        <v>252</v>
+        <v>401</v>
       </c>
       <c r="C393" s="12">
-        <v>86027</v>
+        <v>85995</v>
       </c>
       <c r="D393" s="13">
-        <v>101904</v>
+        <v>85995</v>
       </c>
       <c r="E393" s="14" t="b">
         <v>1</v>
@@ -30746,7 +30754,7 @@
       </c>
       <c r="K393" t="str">
         <f t="shared" si="6"/>
-        <v>[101904] = {true, true, false, false, true, true}, --Fetcher Infection</v>
+        <v>[85995] = {true, true, false, false, true, true}, --Dive</v>
       </c>
     </row>
     <row r="394" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30754,22 +30762,22 @@
         <v>93</v>
       </c>
       <c r="B394" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C394" s="12">
-        <v>86165</v>
+        <v>86027</v>
       </c>
       <c r="D394" s="13">
-        <v>88791</v>
+        <v>101904</v>
       </c>
       <c r="E394" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F394" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G394" s="14" t="b">
-        <v>1</v>
+      <c r="F394" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G394" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H394" s="15" t="b">
         <v>0</v>
@@ -30782,7 +30790,7 @@
       </c>
       <c r="K394" t="str">
         <f t="shared" si="6"/>
-        <v>[88791] = {true, false, true, false, true, true}, --Gripping Shards</v>
+        <v>[101904] = {true, true, false, false, true, true}, --Fetcher Infection</v>
       </c>
     </row>
     <row r="395" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30790,22 +30798,22 @@
         <v>93</v>
       </c>
       <c r="B395" s="11" t="s">
-        <v>82</v>
+        <v>253</v>
       </c>
       <c r="C395" s="12">
-        <v>86031</v>
+        <v>86165</v>
       </c>
       <c r="D395" s="13">
-        <v>101944</v>
+        <v>88791</v>
       </c>
       <c r="E395" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F395" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G395" s="15" t="b">
-        <v>0</v>
+      <c r="F395" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G395" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H395" s="15" t="b">
         <v>0</v>
@@ -30818,7 +30826,7 @@
       </c>
       <c r="K395" t="str">
         <f t="shared" si="6"/>
-        <v>[101944] = {true, true, false, false, true, true}, --Growing Swarm</v>
+        <v>[88791] = {true, false, true, false, true, true}, --Gripping Shards</v>
       </c>
     </row>
     <row r="396" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30826,13 +30834,13 @@
         <v>93</v>
       </c>
       <c r="B396" s="11" t="s">
-        <v>254</v>
+        <v>82</v>
       </c>
       <c r="C396" s="12">
-        <v>85990</v>
+        <v>86031</v>
       </c>
       <c r="D396" s="13">
-        <v>92160</v>
+        <v>101944</v>
       </c>
       <c r="E396" s="14" t="b">
         <v>1</v>
@@ -30854,7 +30862,7 @@
       </c>
       <c r="K396" t="str">
         <f t="shared" si="6"/>
-        <v>[92160] = {true, true, false, false, true, true}, --Guardian Savagery</v>
+        <v>[101944] = {true, true, false, false, true, true}, --Growing Swarm</v>
       </c>
     </row>
     <row r="397" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30862,13 +30870,13 @@
         <v>93</v>
       </c>
       <c r="B397" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C397" s="12">
-        <v>85986</v>
+        <v>85990</v>
       </c>
       <c r="D397" s="13">
-        <v>105921</v>
+        <v>92160</v>
       </c>
       <c r="E397" s="14" t="b">
         <v>1</v>
@@ -30890,7 +30898,7 @@
       </c>
       <c r="K397" t="str">
         <f t="shared" si="6"/>
-        <v>[105921] = {true, true, false, false, true, true}, --Guardian's Wrath (pet)</v>
+        <v>[92160] = {true, true, false, false, true, true}, --Guardian Savagery</v>
       </c>
     </row>
     <row r="398" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30901,10 +30909,10 @@
         <v>255</v>
       </c>
       <c r="C398" s="12">
-        <v>85982</v>
+        <v>85986</v>
       </c>
       <c r="D398" s="13">
-        <v>91974</v>
+        <v>105921</v>
       </c>
       <c r="E398" s="14" t="b">
         <v>1</v>
@@ -30926,7 +30934,7 @@
       </c>
       <c r="K398" t="str">
         <f t="shared" si="6"/>
-        <v>[91974] = {true, true, false, false, true, true}, --Guardian's Wrath (pet)</v>
+        <v>[105921] = {true, true, false, false, true, true}, --Guardian's Wrath (pet)</v>
       </c>
     </row>
     <row r="399" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30934,22 +30942,22 @@
         <v>93</v>
       </c>
       <c r="B399" s="11" t="s">
-        <v>402</v>
+        <v>255</v>
       </c>
       <c r="C399" s="12">
-        <v>86161</v>
+        <v>85982</v>
       </c>
       <c r="D399" s="13">
-        <v>88783</v>
+        <v>91974</v>
       </c>
       <c r="E399" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F399" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G399" s="14" t="b">
-        <v>1</v>
+      <c r="F399" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G399" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H399" s="15" t="b">
         <v>0</v>
@@ -30962,7 +30970,7 @@
       </c>
       <c r="K399" t="str">
         <f t="shared" si="6"/>
-        <v>[88783] = {true, false, true, false, true, true}, --Impaling Shards</v>
+        <v>[91974] = {true, true, false, false, true, true}, --Guardian's Wrath (pet)</v>
       </c>
     </row>
     <row r="400" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30970,13 +30978,13 @@
         <v>93</v>
       </c>
       <c r="B400" s="11" t="s">
-        <v>83</v>
+        <v>402</v>
       </c>
       <c r="C400" s="12">
-        <v>86113</v>
+        <v>86161</v>
       </c>
       <c r="D400" s="13">
-        <v>88860</v>
+        <v>88783</v>
       </c>
       <c r="E400" s="14" t="b">
         <v>1</v>
@@ -30998,7 +31006,7 @@
       </c>
       <c r="K400" t="str">
         <f t="shared" si="6"/>
-        <v>[88860] = {true, false, true, false, true, true}, --Northern Storm</v>
+        <v>[88783] = {true, false, true, false, true, true}, --Impaling Shards</v>
       </c>
     </row>
     <row r="401" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31006,22 +31014,22 @@
         <v>93</v>
       </c>
       <c r="B401" s="11" t="s">
-        <v>256</v>
+        <v>83</v>
       </c>
       <c r="C401" s="12">
-        <v>86117</v>
+        <v>86113</v>
       </c>
       <c r="D401" s="13">
-        <v>88863</v>
+        <v>88860</v>
       </c>
       <c r="E401" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F401" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G401" s="15" t="b">
-        <v>0</v>
+      <c r="F401" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G401" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H401" s="15" t="b">
         <v>0</v>
@@ -31034,7 +31042,7 @@
       </c>
       <c r="K401" t="str">
         <f t="shared" si="6"/>
-        <v>[88863] = {true, true, false, false, true, true}, --Permafrost</v>
+        <v>[88860] = {true, false, true, false, true, true}, --Northern Storm</v>
       </c>
     </row>
     <row r="402" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31042,13 +31050,13 @@
         <v>93</v>
       </c>
       <c r="B402" s="11" t="s">
-        <v>403</v>
+        <v>256</v>
       </c>
       <c r="C402" s="12">
-        <v>86009</v>
+        <v>86117</v>
       </c>
       <c r="D402" s="13">
-        <v>94411</v>
+        <v>88863</v>
       </c>
       <c r="E402" s="14" t="b">
         <v>1</v>
@@ -31070,7 +31078,7 @@
       </c>
       <c r="K402" t="str">
         <f t="shared" si="6"/>
-        <v>[94411] = {true, true, false, false, true, true}, --Scorch</v>
+        <v>[88863] = {true, true, false, false, true, true}, --Permafrost</v>
       </c>
     </row>
     <row r="403" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31078,13 +31086,13 @@
         <v>93</v>
       </c>
       <c r="B403" s="11" t="s">
-        <v>84</v>
+        <v>403</v>
       </c>
       <c r="C403" s="12">
-        <v>86003</v>
+        <v>86009</v>
       </c>
       <c r="D403" s="13">
-        <v>86003</v>
+        <v>94411</v>
       </c>
       <c r="E403" s="14" t="b">
         <v>1</v>
@@ -31106,7 +31114,7 @@
       </c>
       <c r="K403" t="str">
         <f t="shared" si="6"/>
-        <v>[86003] = {true, true, false, false, true, true}, --Screaming Cliff Racer</v>
+        <v>[94411] = {true, true, false, false, true, true}, --Scorch</v>
       </c>
     </row>
     <row r="404" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31114,22 +31122,22 @@
         <v>93</v>
       </c>
       <c r="B404" s="11" t="s">
-        <v>404</v>
+        <v>84</v>
       </c>
       <c r="C404" s="12">
-        <v>86109</v>
+        <v>86003</v>
       </c>
       <c r="D404" s="13">
-        <v>86247</v>
+        <v>86003</v>
       </c>
       <c r="E404" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F404" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G404" s="14" t="b">
-        <v>1</v>
+      <c r="F404" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G404" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H404" s="15" t="b">
         <v>0</v>
@@ -31142,7 +31150,7 @@
       </c>
       <c r="K404" t="str">
         <f t="shared" si="6"/>
-        <v>[86247] = {true, false, true, false, true, true}, --Sleet Storm</v>
+        <v>[86003] = {true, true, false, false, true, true}, --Screaming Cliff Racer</v>
       </c>
     </row>
     <row r="405" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31150,22 +31158,22 @@
         <v>93</v>
       </c>
       <c r="B405" s="11" t="s">
-        <v>257</v>
+        <v>404</v>
       </c>
       <c r="C405" s="12">
-        <v>86019</v>
+        <v>86109</v>
       </c>
       <c r="D405" s="13">
-        <v>94445</v>
+        <v>86247</v>
       </c>
       <c r="E405" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F405" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G405" s="15" t="b">
-        <v>0</v>
+      <c r="F405" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G405" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H405" s="15" t="b">
         <v>0</v>
@@ -31178,7 +31186,7 @@
       </c>
       <c r="K405" t="str">
         <f t="shared" si="6"/>
-        <v>[94445] = {true, true, false, false, true, true}, --Subterranean Assault</v>
+        <v>[86247] = {true, false, true, false, true, true}, --Sleet Storm</v>
       </c>
     </row>
     <row r="406" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31186,22 +31194,22 @@
         <v>93</v>
       </c>
       <c r="B406" s="11" t="s">
-        <v>405</v>
+        <v>257</v>
       </c>
       <c r="C406" s="12">
-        <v>86023</v>
+        <v>86019</v>
       </c>
       <c r="D406" s="13">
-        <v>101703</v>
+        <v>94445</v>
       </c>
       <c r="E406" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F406" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G406" s="14" t="b">
-        <v>1</v>
+      <c r="F406" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G406" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H406" s="15" t="b">
         <v>0</v>
@@ -31214,7 +31222,7 @@
       </c>
       <c r="K406" t="str">
         <f t="shared" si="6"/>
-        <v>[101703] = {true, false, true, false, true, true}, --Swarm</v>
+        <v>[94445] = {true, true, false, false, true, true}, --Subterranean Assault</v>
       </c>
     </row>
     <row r="407" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31222,22 +31230,22 @@
         <v>93</v>
       </c>
       <c r="B407" s="11" t="s">
-        <v>258</v>
+        <v>405</v>
       </c>
       <c r="C407" s="12">
-        <v>85986</v>
+        <v>86023</v>
       </c>
       <c r="D407" s="13">
-        <v>105906</v>
+        <v>101703</v>
       </c>
       <c r="E407" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F407" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G407" s="15" t="b">
-        <v>0</v>
+      <c r="F407" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G407" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H407" s="15" t="b">
         <v>0</v>
@@ -31250,7 +31258,7 @@
       </c>
       <c r="K407" t="str">
         <f t="shared" si="6"/>
-        <v>[105906] = {true, true, false, false, true, true}, --Swipe (pet)</v>
+        <v>[101703] = {true, false, true, false, true, true}, --Swarm</v>
       </c>
     </row>
     <row r="408" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31261,10 +31269,10 @@
         <v>258</v>
       </c>
       <c r="C408" s="12">
-        <v>85982</v>
+        <v>85986</v>
       </c>
       <c r="D408" s="13">
-        <v>89135</v>
+        <v>105906</v>
       </c>
       <c r="E408" s="14" t="b">
         <v>1</v>
@@ -31286,7 +31294,7 @@
       </c>
       <c r="K408" t="str">
         <f t="shared" si="6"/>
-        <v>[89135] = {true, true, false, false, true, true}, --Swipe (pet)</v>
+        <v>[105906] = {true, true, false, false, true, true}, --Swipe (pet)</v>
       </c>
     </row>
     <row r="409" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31297,10 +31305,10 @@
         <v>258</v>
       </c>
       <c r="C409" s="12">
-        <v>85990</v>
+        <v>85982</v>
       </c>
       <c r="D409" s="13">
-        <v>89219</v>
+        <v>89135</v>
       </c>
       <c r="E409" s="14" t="b">
         <v>1</v>
@@ -31322,7 +31330,7 @@
       </c>
       <c r="K409" t="str">
         <f t="shared" si="6"/>
-        <v>[89219] = {true, true, false, false, true, true}, --Swipe (pet)</v>
+        <v>[89135] = {true, true, false, false, true, true}, --Swipe (pet)</v>
       </c>
     </row>
     <row r="410" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31330,22 +31338,22 @@
         <v>93</v>
       </c>
       <c r="B410" s="11" t="s">
-        <v>85</v>
+        <v>258</v>
       </c>
       <c r="C410" s="12">
-        <v>86169</v>
+        <v>85990</v>
       </c>
       <c r="D410" s="13">
-        <v>88802</v>
+        <v>89219</v>
       </c>
       <c r="E410" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F410" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G410" s="14" t="b">
-        <v>1</v>
+      <c r="F410" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G410" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H410" s="15" t="b">
         <v>0</v>
@@ -31358,30 +31366,30 @@
       </c>
       <c r="K410" t="str">
         <f t="shared" si="6"/>
-        <v>[88802] = {true, false, true, false, true, true}, --Winters Revenge</v>
+        <v>[89219] = {true, true, false, false, true, true}, --Swipe (pet)</v>
       </c>
     </row>
     <row r="411" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A411" s="10" t="s">
-        <v>406</v>
+        <v>93</v>
       </c>
       <c r="B411" s="11" t="s">
-        <v>414</v>
+        <v>85</v>
       </c>
       <c r="C411" s="12">
-        <v>39105</v>
+        <v>86169</v>
       </c>
       <c r="D411" s="13">
-        <v>39109</v>
+        <v>88802</v>
       </c>
       <c r="E411" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F411" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G411" s="15" t="b">
-        <v>0</v>
+      <c r="F411" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G411" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H411" s="15" t="b">
         <v>0</v>
@@ -31394,7 +31402,7 @@
       </c>
       <c r="K411" t="str">
         <f t="shared" si="6"/>
-        <v>[39109] = {true, true, false, false, true, true}, --Brutal Pounce</v>
+        <v>[88802] = {true, false, true, false, true, true}, --Winters Revenge</v>
       </c>
     </row>
     <row r="412" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31402,13 +31410,13 @@
         <v>406</v>
       </c>
       <c r="B412" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C412" s="12">
-        <v>58864</v>
+        <v>39105</v>
       </c>
       <c r="D412" s="13">
-        <v>58864</v>
+        <v>39109</v>
       </c>
       <c r="E412" s="14" t="b">
         <v>1</v>
@@ -31430,7 +31438,7 @@
       </c>
       <c r="K412" t="str">
         <f t="shared" si="6"/>
-        <v>[58864] = {true, true, false, false, true, true}, --Claws of Anguish</v>
+        <v>[39109] = {true, true, false, false, true, true}, --Brutal Pounce</v>
       </c>
     </row>
     <row r="413" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31438,13 +31446,13 @@
         <v>406</v>
       </c>
       <c r="B413" s="11" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C413" s="12">
-        <v>58879</v>
+        <v>58864</v>
       </c>
       <c r="D413" s="13">
-        <v>58879</v>
+        <v>58864</v>
       </c>
       <c r="E413" s="14" t="b">
         <v>1</v>
@@ -31466,7 +31474,7 @@
       </c>
       <c r="K413" t="str">
         <f t="shared" si="6"/>
-        <v>[58879] = {true, true, false, false, true, true}, --Claws of Life</v>
+        <v>[58864] = {true, true, false, false, true, true}, --Claws of Anguish</v>
       </c>
     </row>
     <row r="414" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31474,13 +31482,13 @@
         <v>406</v>
       </c>
       <c r="B414" s="11" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C414" s="12">
-        <v>39104</v>
+        <v>58879</v>
       </c>
       <c r="D414" s="13">
-        <v>39107</v>
+        <v>58879</v>
       </c>
       <c r="E414" s="14" t="b">
         <v>1</v>
@@ -31502,7 +31510,7 @@
       </c>
       <c r="K414" t="str">
         <f t="shared" si="6"/>
-        <v>[39107] = {true, true, false, false, true, true}, --Feral Pounce</v>
+        <v>[58879] = {true, true, false, false, true, true}, --Claws of Life</v>
       </c>
     </row>
     <row r="415" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31510,13 +31518,13 @@
         <v>406</v>
       </c>
       <c r="B415" s="11" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C415" s="12">
-        <v>39075</v>
+        <v>39104</v>
       </c>
       <c r="D415" s="13">
-        <v>80189</v>
+        <v>39107</v>
       </c>
       <c r="E415" s="14" t="b">
         <v>1</v>
@@ -31538,7 +31546,7 @@
       </c>
       <c r="K415" t="str">
         <f t="shared" si="6"/>
-        <v>[80189] = {true, true, false, false, true, true}, --Gnash (Pact Leader)</v>
+        <v>[39107] = {true, true, false, false, true, true}, --Feral Pounce</v>
       </c>
     </row>
     <row r="416" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31552,7 +31560,7 @@
         <v>39075</v>
       </c>
       <c r="D416" s="13">
-        <v>80190</v>
+        <v>80189</v>
       </c>
       <c r="E416" s="14" t="b">
         <v>1</v>
@@ -31574,7 +31582,7 @@
       </c>
       <c r="K416" t="str">
         <f t="shared" si="6"/>
-        <v>[80190] = {true, true, false, false, true, true}, --Gnash (Pact Leader)</v>
+        <v>[80189] = {true, true, false, false, true, true}, --Gnash (Pact Leader)</v>
       </c>
     </row>
     <row r="417" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31582,13 +31590,13 @@
         <v>406</v>
       </c>
       <c r="B417" s="11" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C417" s="12">
-        <v>32477</v>
+        <v>39075</v>
       </c>
       <c r="D417" s="13">
-        <v>32494</v>
+        <v>80190</v>
       </c>
       <c r="E417" s="14" t="b">
         <v>1</v>
@@ -31599,8 +31607,8 @@
       <c r="G417" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H417" s="14" t="b">
-        <v>1</v>
+      <c r="H417" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="I417" s="14" t="b">
         <v>1</v>
@@ -31610,7 +31618,7 @@
       </c>
       <c r="K417" t="str">
         <f t="shared" si="6"/>
-        <v>[32494] = {true, true, false, true, true, true}, --Heavy Attack (Splash)</v>
+        <v>[80190] = {true, true, false, false, true, true}, --Gnash (Pact Leader)</v>
       </c>
     </row>
     <row r="418" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31618,13 +31626,13 @@
         <v>406</v>
       </c>
       <c r="B418" s="11" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="C418" s="12">
         <v>32477</v>
       </c>
       <c r="D418" s="13">
-        <v>32480</v>
+        <v>32494</v>
       </c>
       <c r="E418" s="14" t="b">
         <v>1</v>
@@ -31646,7 +31654,7 @@
       </c>
       <c r="K418" t="str">
         <f t="shared" si="6"/>
-        <v>[32480] = {true, true, false, true, true, true}, --Heavy Attack Werewolf</v>
+        <v>[32494] = {true, true, false, true, true, true}, --Heavy Attack (Splash)</v>
       </c>
     </row>
     <row r="419" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31654,13 +31662,13 @@
         <v>406</v>
       </c>
       <c r="B419" s="11" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C419" s="12">
-        <v>58798</v>
+        <v>32477</v>
       </c>
       <c r="D419" s="13">
-        <v>58798</v>
+        <v>32480</v>
       </c>
       <c r="E419" s="14" t="b">
         <v>1</v>
@@ -31671,8 +31679,8 @@
       <c r="G419" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H419" s="15" t="b">
-        <v>0</v>
+      <c r="H419" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="I419" s="14" t="b">
         <v>1</v>
@@ -31682,7 +31690,7 @@
       </c>
       <c r="K419" t="str">
         <f t="shared" si="6"/>
-        <v>[58798] = {true, true, false, false, true, true}, --Howl of Agony</v>
+        <v>[32480] = {true, true, false, true, true, true}, --Heavy Attack Werewolf</v>
       </c>
     </row>
     <row r="420" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31690,13 +31698,13 @@
         <v>406</v>
       </c>
       <c r="B420" s="11" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C420" s="12">
-        <v>58742</v>
+        <v>58798</v>
       </c>
       <c r="D420" s="13">
-        <v>58742</v>
+        <v>58798</v>
       </c>
       <c r="E420" s="14" t="b">
         <v>1</v>
@@ -31718,7 +31726,7 @@
       </c>
       <c r="K420" t="str">
         <f t="shared" si="6"/>
-        <v>[58742] = {true, true, false, false, true, true}, --Howl of Dispair</v>
+        <v>[58798] = {true, true, false, false, true, true}, --Howl of Agony</v>
       </c>
     </row>
     <row r="421" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31726,35 +31734,35 @@
         <v>406</v>
       </c>
       <c r="B421" s="11" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C421" s="12">
-        <v>58855</v>
+        <v>58742</v>
       </c>
       <c r="D421" s="13">
-        <v>58856</v>
+        <v>58742</v>
       </c>
       <c r="E421" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F421" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G421" s="14" t="b">
-        <v>1</v>
+      <c r="F421" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G421" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H421" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="I421" s="15" t="b">
-        <v>0</v>
+      <c r="I421" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="J421" s="14" t="b">
         <v>1</v>
       </c>
       <c r="K421" t="str">
         <f t="shared" si="6"/>
-        <v>[58856] = {true, false, true, false, false, true}, --Infection</v>
+        <v>[58742] = {true, true, false, false, true, true}, --Howl of Dispair</v>
       </c>
     </row>
     <row r="422" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31762,35 +31770,35 @@
         <v>406</v>
       </c>
       <c r="B422" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C422" s="12">
         <v>58855</v>
       </c>
       <c r="D422" s="13">
-        <v>58855</v>
+        <v>58856</v>
       </c>
       <c r="E422" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F422" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G422" s="15" t="b">
-        <v>0</v>
+      <c r="F422" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G422" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H422" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="I422" s="14" t="b">
-        <v>1</v>
+      <c r="I422" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="J422" s="14" t="b">
         <v>1</v>
       </c>
       <c r="K422" t="str">
         <f t="shared" si="6"/>
-        <v>[58855] = {true, true, false, false, true, true}, --Infectious Claws</v>
+        <v>[58856] = {true, false, true, false, false, true}, --Infection</v>
       </c>
     </row>
     <row r="423" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31798,13 +31806,13 @@
         <v>406</v>
       </c>
       <c r="B423" s="11" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C423" s="12">
-        <v>32464</v>
+        <v>58855</v>
       </c>
       <c r="D423" s="13">
-        <v>32464</v>
+        <v>58855</v>
       </c>
       <c r="E423" s="14" t="b">
         <v>1</v>
@@ -31815,8 +31823,8 @@
       <c r="G423" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H423" s="14" t="b">
-        <v>1</v>
+      <c r="H423" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="I423" s="14" t="b">
         <v>1</v>
@@ -31826,7 +31834,7 @@
       </c>
       <c r="K423" t="str">
         <f t="shared" si="6"/>
-        <v>[32464] = {true, true, false, true, true, true}, --Light Attack</v>
+        <v>[58855] = {true, true, false, false, true, true}, --Infectious Claws</v>
       </c>
     </row>
     <row r="424" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31834,13 +31842,13 @@
         <v>406</v>
       </c>
       <c r="B424" s="11" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C424" s="12">
-        <v>39075</v>
+        <v>32464</v>
       </c>
       <c r="D424" s="13">
-        <v>80184</v>
+        <v>32464</v>
       </c>
       <c r="E424" s="14" t="b">
         <v>1</v>
@@ -31851,8 +31859,8 @@
       <c r="G424" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="H424" s="15" t="b">
-        <v>0</v>
+      <c r="H424" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="I424" s="14" t="b">
         <v>1</v>
@@ -31862,7 +31870,7 @@
       </c>
       <c r="K424" t="str">
         <f t="shared" si="6"/>
-        <v>[80184] = {true, true, false, false, true, true}, --Lunge (Pact Leader)</v>
+        <v>[32464] = {true, true, false, true, true, true}, --Light Attack</v>
       </c>
     </row>
     <row r="425" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31870,13 +31878,13 @@
         <v>406</v>
       </c>
       <c r="B425" s="11" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C425" s="12">
-        <v>58405</v>
+        <v>39075</v>
       </c>
       <c r="D425" s="13">
-        <v>58405</v>
+        <v>80184</v>
       </c>
       <c r="E425" s="14" t="b">
         <v>1</v>
@@ -31898,7 +31906,7 @@
       </c>
       <c r="K425" t="str">
         <f t="shared" si="6"/>
-        <v>[58405] = {true, true, false, false, true, true}, --Piercing Howl</v>
+        <v>[80184] = {true, true, false, false, true, true}, --Lunge (Pact Leader)</v>
       </c>
     </row>
     <row r="426" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31906,13 +31914,13 @@
         <v>406</v>
       </c>
       <c r="B426" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C426" s="12">
-        <v>32632</v>
+        <v>58405</v>
       </c>
       <c r="D426" s="13">
-        <v>32645</v>
+        <v>58405</v>
       </c>
       <c r="E426" s="14" t="b">
         <v>1</v>
@@ -31934,7 +31942,7 @@
       </c>
       <c r="K426" t="str">
         <f t="shared" si="6"/>
-        <v>[32645] = {true, true, false, false, true, true}, --Pounce</v>
+        <v>[58405] = {true, true, false, false, true, true}, --Piercing Howl</v>
       </c>
     </row>
     <row r="427" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31942,22 +31950,22 @@
         <v>406</v>
       </c>
       <c r="B427" s="11" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="C427" s="12">
-        <v>32464</v>
+        <v>32632</v>
       </c>
       <c r="D427" s="13">
-        <v>89147</v>
+        <v>32645</v>
       </c>
       <c r="E427" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F427" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G427" s="14" t="b">
-        <v>1</v>
+      <c r="F427" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G427" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="H427" s="15" t="b">
         <v>0</v>
@@ -31965,12 +31973,12 @@
       <c r="I427" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J427" s="15" t="b">
-        <v>0</v>
+      <c r="J427" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="K427" t="str">
         <f t="shared" si="6"/>
-        <v>[89147] = {true, false, true, false, true, false}, --Werewolf Berserker Bleed</v>
+        <v>[32645] = {true, true, false, false, true, true}, --Pounce</v>
       </c>
     </row>
     <row r="428" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31978,13 +31986,13 @@
         <v>406</v>
       </c>
       <c r="B428" s="11" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="C428" s="12">
         <v>32464</v>
       </c>
       <c r="D428" s="13">
-        <v>89146</v>
+        <v>89147</v>
       </c>
       <c r="E428" s="14" t="b">
         <v>1</v>
@@ -32006,30 +32014,30 @@
       </c>
       <c r="K428" t="str">
         <f t="shared" si="6"/>
-        <v>[89146] = {true, false, true, false, true, false}, --Werewolf Bleed</v>
+        <v>[89147] = {true, false, true, false, true, false}, --Werewolf Berserker Bleed</v>
       </c>
     </row>
     <row r="429" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="10" t="s">
-        <v>140</v>
+        <v>406</v>
       </c>
       <c r="B429" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="C429" s="12" t="s">
-        <v>33</v>
+        <v>413</v>
+      </c>
+      <c r="C429" s="12">
+        <v>32464</v>
       </c>
       <c r="D429" s="13">
-        <v>21970</v>
+        <v>89146</v>
       </c>
       <c r="E429" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F429" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G429" s="15" t="b">
-        <v>0</v>
+      <c r="F429" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G429" s="14" t="b">
+        <v>1</v>
       </c>
       <c r="H429" s="15" t="b">
         <v>0</v>
@@ -32037,26 +32045,26 @@
       <c r="I429" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="J429" s="14" t="b">
-        <v>1</v>
+      <c r="J429" s="15" t="b">
+        <v>0</v>
       </c>
       <c r="K429" t="str">
         <f t="shared" si="6"/>
-        <v>[21970] = {true, true, false, false, true, true}, --Bash</v>
+        <v>[89146] = {true, false, true, false, true, false}, --Werewolf Bleed</v>
       </c>
     </row>
     <row r="430" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="10" t="s">
-        <v>465</v>
+        <v>140</v>
       </c>
       <c r="B430" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="C430" s="12">
-        <v>103878</v>
+        <v>471</v>
+      </c>
+      <c r="C430" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D430" s="13">
-        <v>103881</v>
+        <v>21970</v>
       </c>
       <c r="E430" s="14" t="b">
         <v>1</v>
@@ -32078,7 +32086,7 @@
       </c>
       <c r="K430" t="str">
         <f t="shared" si="6"/>
-        <v>[103881] = {true, true, false, false, true, true}, --Spell Orb (physical)</v>
+        <v>[21970] = {true, true, false, false, true, true}, --Bash</v>
       </c>
     </row>
     <row r="431" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32086,13 +32094,13 @@
         <v>465</v>
       </c>
       <c r="B431" s="11" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="C431" s="12">
-        <v>103483</v>
+        <v>103878</v>
       </c>
       <c r="D431" s="13">
-        <v>103485</v>
+        <v>103881</v>
       </c>
       <c r="E431" s="14" t="b">
         <v>1</v>
@@ -32114,7 +32122,7 @@
       </c>
       <c r="K431" t="str">
         <f t="shared" si="6"/>
-        <v>[103485] = {true, true, false, false, true, true}, --Imbue Weapon</v>
+        <v>[103881] = {true, true, false, false, true, true}, --Spell Orb (physical)</v>
       </c>
     </row>
     <row r="432" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32122,13 +32130,13 @@
         <v>465</v>
       </c>
       <c r="B432" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C432" s="12">
-        <v>103571</v>
+        <v>103483</v>
       </c>
       <c r="D432" s="13">
-        <v>103572</v>
+        <v>103485</v>
       </c>
       <c r="E432" s="14" t="b">
         <v>1</v>
@@ -32150,7 +32158,7 @@
       </c>
       <c r="K432" t="str">
         <f t="shared" si="6"/>
-        <v>[103572] = {true, true, false, false, true, true}, --Elemental Weapon</v>
+        <v>[103485] = {true, true, false, false, true, true}, --Imbue Weapon</v>
       </c>
     </row>
     <row r="433" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32158,13 +32166,13 @@
         <v>465</v>
       </c>
       <c r="B433" s="11" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C433" s="12">
-        <v>103623</v>
+        <v>103571</v>
       </c>
       <c r="D433" s="13">
-        <v>103626</v>
+        <v>103572</v>
       </c>
       <c r="E433" s="14" t="b">
         <v>1</v>
@@ -32186,7 +32194,7 @@
       </c>
       <c r="K433" t="str">
         <f t="shared" si="6"/>
-        <v>[103626] = {true, true, false, false, true, true}, --Crushing Weapon</v>
+        <v>[103572] = {true, true, false, false, true, true}, --Elemental Weapon</v>
       </c>
     </row>
     <row r="434" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -32194,13 +32202,13 @@
         <v>465</v>
       </c>
       <c r="B434" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C434" s="12">
-        <v>103878</v>
+        <v>103623</v>
       </c>
       <c r="D434" s="13">
-        <v>103880</v>
+        <v>103626</v>
       </c>
       <c r="E434" s="14" t="b">
         <v>1</v>
@@ -32222,21 +32230,21 @@
       </c>
       <c r="K434" t="str">
         <f t="shared" si="6"/>
-        <v>[103880] = {true, true, false, false, true, true}, --Spell Orb (magic)</v>
+        <v>[103626] = {true, true, false, false, true, true}, --Crushing Weapon</v>
       </c>
     </row>
     <row r="435" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A435" s="10" t="s">
-        <v>140</v>
+        <v>465</v>
       </c>
       <c r="B435" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="C435" s="12" t="s">
-        <v>33</v>
+        <v>469</v>
+      </c>
+      <c r="C435" s="12">
+        <v>103878</v>
       </c>
       <c r="D435" s="13">
-        <v>60230</v>
+        <v>103880</v>
       </c>
       <c r="E435" s="14" t="b">
         <v>1</v>
@@ -32258,20 +32266,44 @@
       </c>
       <c r="K435" t="str">
         <f t="shared" si="6"/>
+        <v>[103880] = {true, true, false, false, true, true}, --Spell Orb (magic)</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A436" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B436" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="C436" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D436" s="13">
+        <v>60230</v>
+      </c>
+      <c r="E436" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F436" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G436" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H436" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I436" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J436" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K436" t="str">
+        <f t="shared" si="6"/>
         <v>[60230] = {true, true, false, false, true, true}, --Riposte</v>
       </c>
-    </row>
-    <row r="436" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A436" s="16"/>
-      <c r="B436" s="16"/>
-      <c r="C436" s="16"/>
-      <c r="D436" s="27"/>
-      <c r="E436" s="16"/>
-      <c r="F436" s="16"/>
-      <c r="G436" s="16"/>
-      <c r="H436" s="16"/>
-      <c r="I436" s="16"/>
-      <c r="J436" s="16"/>
     </row>
     <row r="437" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A437" s="16"/>

</xml_diff>

<commit_message>
Updated a few abilities Removed bundled Libraries. Removed unnecessary white spaces. Fixed leaking globals minor fixes in XML code
</commit_message>
<xml_diff>
--- a/CPData.xlsx
+++ b/CPData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk-mi\Documents\ESOdev\Constellations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA42B6F-43E4-41E0-B130-40E837FECE95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F45AE4-91C2-4B5C-A4AE-A543593D76AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2040" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion Table" sheetId="1" r:id="rId1"/>
@@ -1904,7 +1904,91 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -10572,8 +10656,8 @@
   <dimension ref="A1:R585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L425" sqref="L425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16424,24 +16508,14 @@
       <c r="D114" s="11">
         <v>38857</v>
       </c>
-      <c r="E114" s="9">
-        <v>336</v>
-      </c>
-      <c r="F114" s="9">
-        <v>626</v>
-      </c>
-      <c r="G114" s="13">
-        <f>F114/E114/N$2/1.52-1</f>
-        <v>8.9986396360027587E-2</v>
-      </c>
       <c r="H114" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I114" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K114" s="9" t="s">
         <v>347</v>
@@ -16460,7 +16534,7 @@
       </c>
       <c r="R114" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>[38857] = {true, false, true, false, true, true}, --Rapid Strikes</v>
+        <v>[38857] = {true, true, false, false, true, true}, --Rapid Strikes</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
@@ -20134,7 +20208,7 @@
         <v>346</v>
       </c>
       <c r="I187" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J187" s="9" t="s">
         <v>346</v>
@@ -20143,7 +20217,7 @@
         <v>347</v>
       </c>
       <c r="L187" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M187" s="9" t="s">
         <v>346</v>
@@ -20159,7 +20233,7 @@
       </c>
       <c r="R187" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>[107203] = {true, true, true, false, true, true}, --Arms of Relequen</v>
+        <v>[107203] = {true, false, true, false, false, true}, --Arms of Relequen</v>
       </c>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
@@ -31720,7 +31794,7 @@
         <v>347</v>
       </c>
       <c r="L425" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M425" s="9" t="s">
         <v>347</v>
@@ -31728,7 +31802,7 @@
       <c r="P425" s="12"/>
       <c r="R425" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[26411] = {false, false, false, false, false, false}, --Backlash</v>
+        <v>[26411] = {false, false, false, false, true, false}, --Backlash</v>
       </c>
     </row>
     <row r="426" spans="1:18" x14ac:dyDescent="0.25">
@@ -31846,24 +31920,14 @@
       <c r="D428" s="11">
         <v>26794</v>
       </c>
-      <c r="E428" s="9">
-        <v>251</v>
-      </c>
-      <c r="F428" s="9">
-        <v>466</v>
-      </c>
-      <c r="G428" s="13">
-        <f>F428/E428/N$2/1.52-1</f>
-        <v>8.6171034688515391E-2</v>
-      </c>
       <c r="H428" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I428" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J428" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K428" s="9" t="s">
         <v>347</v>
@@ -31882,7 +31946,7 @@
       </c>
       <c r="R428" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[26794] = {true, false, true, false, true, true}, --Biting Jabs</v>
+        <v>[26794] = {true, true, false, false, true, true}, --Biting Jabs</v>
       </c>
     </row>
     <row r="429" spans="1:18" x14ac:dyDescent="0.25">
@@ -31899,24 +31963,14 @@
       <c r="D429" s="11">
         <v>44432</v>
       </c>
-      <c r="E429" s="9">
-        <v>642</v>
-      </c>
-      <c r="F429" s="9">
-        <v>1196</v>
-      </c>
-      <c r="G429" s="13">
-        <f>F429/E429/N$2/1.52-1</f>
-        <v>8.9888759407142471E-2</v>
-      </c>
       <c r="H429" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I429" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J429" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K429" s="9" t="s">
         <v>347</v>
@@ -31930,7 +31984,7 @@
       <c r="P429" s="12"/>
       <c r="R429" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[44432] = {true, false, true, false, true, true}, --Biting Jabs</v>
+        <v>[44432] = {true, true, false, false, true, true}, --Biting Jabs</v>
       </c>
     </row>
     <row r="430" spans="1:18" x14ac:dyDescent="0.25">
@@ -32770,7 +32824,7 @@
         <v>347</v>
       </c>
       <c r="L446" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M446" s="9" t="s">
         <v>347</v>
@@ -32778,7 +32832,7 @@
       <c r="P446" s="12"/>
       <c r="R446" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[27567] = {false, false, false, false, false, false}, --Power of the Light</v>
+        <v>[27567] = {false, false, false, false, true, false}, --Power of the Light</v>
       </c>
     </row>
     <row r="447" spans="1:18" x14ac:dyDescent="0.25">
@@ -32843,24 +32897,14 @@
       <c r="D448" s="11">
         <v>26116</v>
       </c>
-      <c r="E448" s="9">
-        <v>326</v>
-      </c>
-      <c r="F448" s="9">
-        <v>608</v>
-      </c>
-      <c r="G448" s="13">
-        <f>F448/E448/N$2/1.52-1</f>
-        <v>9.111870548029799E-2</v>
-      </c>
       <c r="H448" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I448" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J448" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K448" s="9" t="s">
         <v>347</v>
@@ -32879,7 +32923,7 @@
       </c>
       <c r="R448" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[26116] = {true, false, true, false, true, true}, --Puncturing Strikes</v>
+        <v>[26116] = {true, true, false, false, true, true}, --Puncturing Strikes</v>
       </c>
     </row>
     <row r="449" spans="1:18" x14ac:dyDescent="0.25">
@@ -32896,24 +32940,14 @@
       <c r="D449" s="11">
         <v>44426</v>
       </c>
-      <c r="E449" s="9">
-        <v>848</v>
-      </c>
-      <c r="F449" s="9">
-        <v>1581</v>
-      </c>
-      <c r="G449" s="13">
-        <f>F449/E449/N$2/1.52-1</f>
-        <v>9.0742008124337747E-2</v>
-      </c>
       <c r="H449" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I449" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J449" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K449" s="9" t="s">
         <v>347</v>
@@ -32932,7 +32966,7 @@
       </c>
       <c r="R449" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[44426] = {true, false, true, false, true, true}, --Puncturing Strikes</v>
+        <v>[44426] = {true, true, false, false, true, true}, --Puncturing Strikes</v>
       </c>
     </row>
     <row r="450" spans="1:18" x14ac:dyDescent="0.25">
@@ -32949,24 +32983,14 @@
       <c r="D450" s="11">
         <v>26799</v>
       </c>
-      <c r="E450" s="9">
-        <v>341</v>
-      </c>
-      <c r="F450" s="9">
-        <v>635</v>
-      </c>
-      <c r="G450" s="13">
-        <f>F450/E450/N$2/1.52-1</f>
-        <v>8.9445145959428984E-2</v>
-      </c>
       <c r="H450" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I450" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J450" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K450" s="9" t="s">
         <v>347</v>
@@ -32985,7 +33009,7 @@
       </c>
       <c r="R450" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>[26799] = {true, false, true, false, true, true}, --Puncturing Sweep</v>
+        <v>[26799] = {true, true, false, false, true, true}, --Puncturing Sweep</v>
       </c>
     </row>
     <row r="451" spans="1:18" x14ac:dyDescent="0.25">
@@ -33002,24 +33026,14 @@
       <c r="D451" s="11">
         <v>44436</v>
       </c>
-      <c r="E451" s="9">
-        <v>877</v>
-      </c>
-      <c r="F451" s="9">
-        <v>1634</v>
-      </c>
-      <c r="G451" s="13">
-        <f>F451/E451/N$2/1.52-1</f>
-        <v>9.0030075072891957E-2</v>
-      </c>
       <c r="H451" s="9" t="s">
         <v>346</v>
       </c>
       <c r="I451" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J451" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K451" s="9" t="s">
         <v>347</v>
@@ -33038,7 +33052,7 @@
       </c>
       <c r="R451" s="9" t="str">
         <f t="shared" ref="R451:R514" si="7">CONCATENATE("[",D451,"] = {",LOWER(H451),", ",LOWER(I451),", ",LOWER(J451),", ",LOWER(K451),", ",LOWER(L451),", ",LOWER(M451),"}, --",B451)</f>
-        <v>[44436] = {true, false, true, false, true, true}, --Puncturing Sweep</v>
+        <v>[44436] = {true, true, false, false, true, true}, --Puncturing Sweep</v>
       </c>
     </row>
     <row r="452" spans="1:18" x14ac:dyDescent="0.25">
@@ -33071,7 +33085,7 @@
         <v>347</v>
       </c>
       <c r="L452" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M452" s="9" t="s">
         <v>347</v>
@@ -33079,7 +33093,7 @@
       <c r="P452" s="12"/>
       <c r="R452" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>[27544] = {false, false, false, false, false, false}, --Purifying Light</v>
+        <v>[27544] = {false, false, false, false, true, false}, --Purifying Light</v>
       </c>
     </row>
     <row r="453" spans="1:18" x14ac:dyDescent="0.25">
@@ -35107,17 +35121,17 @@
         <v>38823</v>
       </c>
       <c r="D492" s="11">
-        <v>38823</v>
+        <v>38827</v>
       </c>
       <c r="E492" s="9">
-        <v>1080</v>
+        <v>446</v>
       </c>
       <c r="F492" s="9">
-        <v>1937</v>
+        <v>900</v>
       </c>
       <c r="G492" s="13">
-        <f>F492/E492/N$2/1.52-1</f>
-        <v>4.9281189083820731E-2</v>
+        <f>F492/E492/N$2/N$2/1.52-1</f>
+        <v>4.9840402930562355E-2</v>
       </c>
       <c r="H492" s="9" t="s">
         <v>346</v>
@@ -35135,17 +35149,17 @@
         <v>346</v>
       </c>
       <c r="M492" s="9" t="s">
-        <v>346</v>
+        <v>519</v>
       </c>
       <c r="P492" s="9" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="Q492" s="9">
-        <v>28448</v>
+        <v>28302</v>
       </c>
       <c r="R492" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>[38823] = {true, true, false, false, true, true}, --Reverse Slice</v>
+        <v>[38827] = {true, true, false, false, true, double}, --Reverse Slice</v>
       </c>
     </row>
     <row r="493" spans="1:18" x14ac:dyDescent="0.25">
@@ -35160,17 +35174,17 @@
         <v>38823</v>
       </c>
       <c r="D493" s="11">
-        <v>38827</v>
+        <v>38823</v>
       </c>
       <c r="E493" s="9">
-        <v>446</v>
+        <v>1080</v>
       </c>
       <c r="F493" s="9">
-        <v>900</v>
+        <v>1937</v>
       </c>
       <c r="G493" s="13">
-        <f>F493/E493/N$2/N$2/1.52-1</f>
-        <v>4.9840402930562355E-2</v>
+        <f>F493/E493/N$2/1.52-1</f>
+        <v>4.9281189083820731E-2</v>
       </c>
       <c r="H493" s="9" t="s">
         <v>346</v>
@@ -35188,17 +35202,17 @@
         <v>346</v>
       </c>
       <c r="M493" s="9" t="s">
-        <v>519</v>
+        <v>346</v>
       </c>
       <c r="P493" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Q493" s="9">
-        <v>28302</v>
+        <v>28448</v>
       </c>
       <c r="R493" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>[38827] = {true, true, false, false, true, double}, --Reverse Slice</v>
+        <v>[38823] = {true, true, false, false, true, true}, --Reverse Slice</v>
       </c>
     </row>
     <row r="494" spans="1:18" x14ac:dyDescent="0.25">
@@ -39050,7 +39064,55 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F349:F353">
     <sortCondition ref="F349"/>
   </sortState>
-  <conditionalFormatting sqref="H440:M440 H463:M463 H470:M489 H491:M493 H518:M518 H507:M512 H515:M516 H491:K496 H1:M106 H520:M557 H567:M1048576 H109:M245 H5:K245 H254:M295 H254:K463 H297:M419">
+  <conditionalFormatting sqref="H440:M440 H463:M463 H470:M489 H491:M493 H518:M518 H507:M512 H515:M516 H491:K496 H1:M106 H520:M557 H567:M1048576 H109:M245 H254:M295 H254:K427 H297:M419 H5:K245 H452:K463 H430:K447">
+    <cfRule type="cellIs" dxfId="167" priority="211" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="212" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H420:M424 H426:M427 H425:K425 M425">
+    <cfRule type="cellIs" dxfId="165" priority="209" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="210" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H441:M441">
+    <cfRule type="cellIs" dxfId="163" priority="207" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="208" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H442 K442:M442">
+    <cfRule type="cellIs" dxfId="161" priority="205" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="206" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I442:J442">
+    <cfRule type="cellIs" dxfId="159" priority="203" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="204" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H446:M447">
+    <cfRule type="cellIs" dxfId="157" priority="201" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="202" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H444:M445">
     <cfRule type="cellIs" dxfId="155" priority="199" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39058,7 +39120,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H420:M428">
+  <conditionalFormatting sqref="H443:M443">
     <cfRule type="cellIs" dxfId="153" priority="197" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39066,95 +39128,79 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H441:M441">
-    <cfRule type="cellIs" dxfId="151" priority="195" operator="equal">
+  <conditionalFormatting sqref="H406:M406">
+    <cfRule type="cellIs" dxfId="151" priority="181" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="196" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H442 K442:M442">
-    <cfRule type="cellIs" dxfId="149" priority="193" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="194" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I442:J442">
-    <cfRule type="cellIs" dxfId="147" priority="191" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="192" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H446:M448">
-    <cfRule type="cellIs" dxfId="145" priority="189" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="190" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H444:M445">
-    <cfRule type="cellIs" dxfId="143" priority="187" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="188" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H443:M443">
-    <cfRule type="cellIs" dxfId="141" priority="185" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="186" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H406:M406">
-    <cfRule type="cellIs" dxfId="139" priority="169" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="182" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H411:M412">
-    <cfRule type="cellIs" dxfId="137" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="179" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="180" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H405:M405">
-    <cfRule type="cellIs" dxfId="135" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="177" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="178" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H407:M410">
-    <cfRule type="cellIs" dxfId="133" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="175" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="176" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H430:M430">
-    <cfRule type="cellIs" dxfId="131" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="171" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="172" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H429:M429">
+  <conditionalFormatting sqref="H431:M432">
+    <cfRule type="cellIs" dxfId="139" priority="167" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="168" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H433:M434">
+    <cfRule type="cellIs" dxfId="137" priority="165" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="166" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H453:M454">
+    <cfRule type="cellIs" dxfId="135" priority="163" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="164" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H452:K452 M452">
+    <cfRule type="cellIs" dxfId="133" priority="161" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="162" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H416:M419">
     <cfRule type="cellIs" dxfId="129" priority="157" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39162,71 +39208,71 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H431:M432">
-    <cfRule type="cellIs" dxfId="127" priority="155" operator="equal">
+  <conditionalFormatting sqref="H437:M439">
+    <cfRule type="cellIs" dxfId="127" priority="153" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="156" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H433:M434">
-    <cfRule type="cellIs" dxfId="125" priority="153" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="154" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H453:M454">
-    <cfRule type="cellIs" dxfId="123" priority="151" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="152" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H449:M449 H451:M452">
-    <cfRule type="cellIs" dxfId="121" priority="149" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="150" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H450:M450">
-    <cfRule type="cellIs" dxfId="119" priority="147" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="148" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H416:M419">
-    <cfRule type="cellIs" dxfId="117" priority="145" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="146" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H437:M439">
-    <cfRule type="cellIs" dxfId="115" priority="141" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="154" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H435:M436">
-    <cfRule type="cellIs" dxfId="113" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="151" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="152" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H455:M455">
+    <cfRule type="cellIs" dxfId="123" priority="149" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="150" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H458:M460">
+    <cfRule type="cellIs" dxfId="121" priority="147" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="148" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H456:M457">
+    <cfRule type="cellIs" dxfId="119" priority="145" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="146" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I461:J461">
+    <cfRule type="cellIs" dxfId="117" priority="135" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="136" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H296:L296">
+    <cfRule type="cellIs" dxfId="115" priority="131" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="132" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H464:M465 H464:K490">
+    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H461 K461:M461">
     <cfRule type="cellIs" dxfId="111" priority="137" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39234,15 +39280,15 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H458:M460">
-    <cfRule type="cellIs" dxfId="109" priority="135" operator="equal">
+  <conditionalFormatting sqref="H473:M473">
+    <cfRule type="cellIs" dxfId="109" priority="129" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="130" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H456:M457">
+  <conditionalFormatting sqref="M296">
     <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39250,55 +39296,55 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I461:J461">
-    <cfRule type="cellIs" dxfId="105" priority="123" operator="equal">
+  <conditionalFormatting sqref="H474:M477">
+    <cfRule type="cellIs" dxfId="105" priority="121" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="122" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H296:L296">
-    <cfRule type="cellIs" dxfId="103" priority="119" operator="equal">
+  <conditionalFormatting sqref="H471:M472">
+    <cfRule type="cellIs" dxfId="103" priority="127" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="128" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H464:M465 H464:K490">
-    <cfRule type="cellIs" dxfId="101" priority="113" operator="equal">
+  <conditionalFormatting sqref="H466:M467">
+    <cfRule type="cellIs" dxfId="101" priority="119" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="120" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H461 K461:M461">
-    <cfRule type="cellIs" dxfId="99" priority="125" operator="equal">
+  <conditionalFormatting sqref="H468:M469">
+    <cfRule type="cellIs" dxfId="99" priority="117" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="118" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H473:M473">
-    <cfRule type="cellIs" dxfId="97" priority="117" operator="equal">
+  <conditionalFormatting sqref="H478:M478">
+    <cfRule type="cellIs" dxfId="97" priority="115" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="116" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M296">
-    <cfRule type="cellIs" dxfId="95" priority="121" operator="equal">
+  <conditionalFormatting sqref="H479:M479">
+    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="114" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H474:M477">
+  <conditionalFormatting sqref="H482:M482">
     <cfRule type="cellIs" dxfId="93" priority="109" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39306,47 +39352,47 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H471:M472">
-    <cfRule type="cellIs" dxfId="91" priority="115" operator="equal">
+  <conditionalFormatting sqref="H476:M476">
+    <cfRule type="cellIs" dxfId="91" priority="107" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="108" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H466:M467">
-    <cfRule type="cellIs" dxfId="89" priority="107" operator="equal">
+  <conditionalFormatting sqref="H481:M481">
+    <cfRule type="cellIs" dxfId="89" priority="105" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="106" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H468:M469">
-    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
+  <conditionalFormatting sqref="H483:M485">
+    <cfRule type="cellIs" dxfId="87" priority="103" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="104" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H478:M478">
-    <cfRule type="cellIs" dxfId="85" priority="103" operator="equal">
+  <conditionalFormatting sqref="H494:M498">
+    <cfRule type="cellIs" dxfId="85" priority="101" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="102" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H479:M479">
-    <cfRule type="cellIs" dxfId="83" priority="101" operator="equal">
+  <conditionalFormatting sqref="H496:M498">
+    <cfRule type="cellIs" dxfId="83" priority="99" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="100" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H482:M482">
+  <conditionalFormatting sqref="H494:M495">
     <cfRule type="cellIs" dxfId="81" priority="97" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39354,55 +39400,55 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H476:M476">
-    <cfRule type="cellIs" dxfId="79" priority="95" operator="equal">
+  <conditionalFormatting sqref="H488:M488">
+    <cfRule type="cellIs" dxfId="79" priority="93" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="94" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H481:M481">
-    <cfRule type="cellIs" dxfId="77" priority="93" operator="equal">
+  <conditionalFormatting sqref="H487:M487">
+    <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="92" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H483:M485">
-    <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
+  <conditionalFormatting sqref="H486:M486">
+    <cfRule type="cellIs" dxfId="75" priority="89" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="90" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H494:M498">
-    <cfRule type="cellIs" dxfId="73" priority="89" operator="equal">
+  <conditionalFormatting sqref="H501:M504">
+    <cfRule type="cellIs" dxfId="73" priority="87" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="88" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H496:M498">
-    <cfRule type="cellIs" dxfId="71" priority="87" operator="equal">
+  <conditionalFormatting sqref="H501:M504">
+    <cfRule type="cellIs" dxfId="71" priority="85" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="86" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H494:M495">
-    <cfRule type="cellIs" dxfId="69" priority="85" operator="equal">
+  <conditionalFormatting sqref="H499:M500">
+    <cfRule type="cellIs" dxfId="69" priority="83" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="84" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H488:M488">
+  <conditionalFormatting sqref="H499:M500">
     <cfRule type="cellIs" dxfId="67" priority="81" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39410,55 +39456,55 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H487:M487">
-    <cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
+  <conditionalFormatting sqref="H505:M506">
+    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="80" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H486:M486">
-    <cfRule type="cellIs" dxfId="63" priority="77" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="78" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H501:M504">
-    <cfRule type="cellIs" dxfId="61" priority="75" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="76" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H501:M504">
-    <cfRule type="cellIs" dxfId="59" priority="73" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="74" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H499:M500">
-    <cfRule type="cellIs" dxfId="57" priority="71" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H499:M500">
-    <cfRule type="cellIs" dxfId="55" priority="69" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H505:M506">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H490:M490">
+    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H490:M490">
+    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H492:M492">
+    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H492:M492">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H512:M512">
     <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39466,7 +39512,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H505:M506">
+  <conditionalFormatting sqref="H512:M512">
     <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39474,7 +39520,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H490:M490">
+  <conditionalFormatting sqref="H519:M519">
     <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39482,7 +39528,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H490:M490">
+  <conditionalFormatting sqref="H519:M519">
     <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39490,7 +39536,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H492:M492">
+  <conditionalFormatting sqref="H517:M517">
     <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39498,7 +39544,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H492:M492">
+  <conditionalFormatting sqref="H517:M517">
     <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39506,23 +39552,23 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H512:M512">
-    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
+  <conditionalFormatting sqref="H521:M522">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="46" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H512:M512">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+  <conditionalFormatting sqref="H521:M522">
+    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="48" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H519:M519">
+  <conditionalFormatting sqref="H513:M513">
     <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39530,7 +39576,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H519:M519">
+  <conditionalFormatting sqref="H513:M513">
     <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39538,39 +39584,39 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H517:M517">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+  <conditionalFormatting sqref="H514:M514">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H517:M517">
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
+  <conditionalFormatting sqref="H514:M514">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H521:M522">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+  <conditionalFormatting sqref="H462:M462">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H521:M522">
-    <cfRule type="cellIs" dxfId="27" priority="35" operator="equal">
+  <conditionalFormatting sqref="H108:M108">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H513:M513">
+  <conditionalFormatting sqref="H107:M107">
     <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39578,79 +39624,79 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H513:M513">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+  <conditionalFormatting sqref="H524:M524">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H514:M514">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H514:M514">
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H462:M462">
-    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108:M108">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H107:M107">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H524:M524">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H524:M524">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H558:M559">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H560:M561">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H562:M566">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H246:M253">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H448:K451">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H448:M451">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H428:K429">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H428:M429">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39658,7 +39704,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H562:M566">
+  <conditionalFormatting sqref="L452">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -39666,7 +39712,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H246:M253">
+  <conditionalFormatting sqref="L425">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>